<commit_message>
Make Dimensions one column
</commit_message>
<xml_diff>
--- a/docs/Extractor interface mapping.xlsx
+++ b/docs/Extractor interface mapping.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emeryr/code/digital-scriptorium/ds-convert/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5F88E0A5-3CFC-D446-8A11-0C9017C58824}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D614087-1923-CE48-8C59-FEEE3E550621}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17440" xr2:uid="{30992FE6-2C28-694C-B1F0-6B67346387D2}"/>
   </bookViews>
@@ -467,9 +467,6 @@
     <t>Acknowledgements</t>
   </si>
   <si>
-    <t>Extractor interace</t>
-  </si>
-  <si>
     <t>N/A -- manifest/mapper</t>
   </si>
   <si>
@@ -501,6 +498,9 @@
   </si>
   <si>
     <t>extract_former_owner_as_recorded_agr xml</t>
+  </si>
+  <si>
+    <t>Extractor interface</t>
   </si>
 </sst>
 </file>
@@ -882,7 +882,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D108" sqref="D108"/>
+      <selection pane="bottomLeft" activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -903,7 +903,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>143</v>
+        <v>154</v>
       </c>
     </row>
     <row r="2" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -923,7 +923,7 @@
         <v>83</v>
       </c>
       <c r="D3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -931,7 +931,7 @@
         <v>118</v>
       </c>
       <c r="D4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -953,7 +953,7 @@
         <v>100</v>
       </c>
       <c r="D6" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -964,7 +964,7 @@
         <v>86</v>
       </c>
       <c r="D7" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -975,7 +975,7 @@
         <v>81</v>
       </c>
       <c r="D8" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -986,7 +986,7 @@
         <v>89</v>
       </c>
       <c r="D9" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -1220,7 +1220,7 @@
         <v>8</v>
       </c>
       <c r="D41" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
@@ -1231,7 +1231,7 @@
         <v>11</v>
       </c>
       <c r="D42" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
@@ -1247,7 +1247,7 @@
         <v>20</v>
       </c>
       <c r="D44" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
@@ -1255,7 +1255,7 @@
         <v>23</v>
       </c>
       <c r="D45" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
@@ -1266,7 +1266,7 @@
         <v>26</v>
       </c>
       <c r="D46" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
@@ -1274,7 +1274,7 @@
         <v>29</v>
       </c>
       <c r="D47" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
@@ -1285,7 +1285,7 @@
         <v>32</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
@@ -1293,7 +1293,7 @@
         <v>35</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>